<commit_message>
fixed theming etc. dropped obsolete stuff.
</commit_message>
<xml_diff>
--- a/spraycalc.xlsx
+++ b/spraycalc.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Statisch" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Dynamisch" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Beispiel" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="17">
   <si>
     <t xml:space="preserve">Liter</t>
   </si>
@@ -60,6 +61,9 @@
   </si>
   <si>
     <t xml:space="preserve">Mittel 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l/h</t>
   </si>
   <si>
     <t xml:space="preserve">Lookup</t>
@@ -84,6 +88,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -105,6 +110,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -173,7 +179,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -182,6 +188,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -190,7 +200,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -286,10 +296,10 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -300,36 +310,36 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="2" t="n">
         <v>2000</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="2" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="2" t="n">
         <f aca="false">B2-B3</f>
         <v>1800</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="4" t="n">
         <f aca="false">C2-C3</f>
         <v>9</v>
       </c>
@@ -341,91 +351,91 @@
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="2" t="n">
         <v>179</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="2" t="n">
         <v>1611</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="2" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="2" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="2" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="2" t="n">
         <v>36</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="2" t="n">
         <v>45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="2" t="n">
         <v>54</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="4" t="n">
         <f aca="false">SUM(B7:B13)</f>
         <v>200</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="2" t="n">
         <f aca="false">SUM(C7:C13)</f>
         <v>1800</v>
       </c>
@@ -446,13 +456,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.37"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -461,40 +474,56 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="2" t="n">
         <v>2000</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="2" t="n">
         <v>10</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <f aca="false">B2/C2</f>
+        <v>200</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="5" t="n">
+        <f aca="false">B3/B2*C2</f>
         <v>1</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">B3/C3</f>
+        <v>200</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="6" t="n">
         <f aca="false">B2-B3</f>
         <v>1800</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="6" t="n">
         <f aca="false">C2-C3</f>
         <v>9</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">B4/C4</f>
+        <v>200</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -506,119 +535,325 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="n">
-        <f aca="false">B3-SUM(B8:B13)</f>
+      <c r="B7" s="6" t="n">
+        <f aca="false">B4/C4-SUM(B8:B13)</f>
         <v>179</v>
       </c>
       <c r="C7" s="5" t="n">
-        <f aca="false">B4-SUM(C8:C13)</f>
+        <f aca="false">B7*$C$4</f>
         <v>1611</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="n">
+      <c r="B8" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="5" t="n">
         <f aca="false">B8*$C$4</f>
         <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="n">
+      <c r="B9" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="5" t="n">
         <f aca="false">B9*$C$4</f>
         <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="n">
+      <c r="B10" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="5" t="n">
         <f aca="false">B10*$C$4</f>
         <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="n">
+      <c r="B11" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" s="5" t="n">
         <f aca="false">B11*$C$4</f>
         <v>36</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="n">
+      <c r="B12" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="5" t="n">
         <f aca="false">B12*$C$4</f>
         <v>45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="n">
+      <c r="B13" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="C13" s="3" t="n">
+      <c r="C13" s="5" t="n">
         <f aca="false">B13*$C$4</f>
         <v>54</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="7" t="n">
+      <c r="B14" s="8" t="n">
         <f aca="false">SUM(B7:B13)</f>
         <v>200</v>
       </c>
-      <c r="C14" s="7" t="n">
+      <c r="C14" s="8" t="n">
         <f aca="false">SUM(C7:C13)</f>
         <v>1800</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
-        <v>13</v>
+      <c r="A18" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
-        <v>14</v>
+      <c r="A19" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
-        <v>15</v>
+      <c r="A20" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.4"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>3300</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>280</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <f aca="false">B2/C2</f>
+        <v>11.7857142857143</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>330</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <f aca="false">B3/B2*C2</f>
+        <v>28</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">B3/C3</f>
+        <v>11.7857142857143</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <f aca="false">B2-B3</f>
+        <v>2970</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <f aca="false">C2-C3</f>
+        <v>252</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">B4/C4</f>
+        <v>11.7857142857143</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <f aca="false">C4-SUM(B8:B13)</f>
+        <v>231</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <f aca="false">B7*$D$4</f>
+        <v>2722.5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <f aca="false">B8*$D$4</f>
+        <v>11.7857142857143</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <f aca="false">B9*$D$4</f>
+        <v>23.5714285714286</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" s="5" t="n">
+        <f aca="false">B10*$D$4</f>
+        <v>35.3571428571429</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <f aca="false">B11*$D$4</f>
+        <v>47.1428571428571</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C12" s="5" t="n">
+        <f aca="false">B12*$D$4</f>
+        <v>58.9285714285714</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C13" s="5" t="n">
+        <f aca="false">B13*$D$4</f>
+        <v>70.7142857142857</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="8" t="n">
+        <f aca="false">SUM(B7:B13)</f>
+        <v>252</v>
+      </c>
+      <c r="C14" s="8" t="n">
+        <f aca="false">SUM(C7:C13)</f>
+        <v>2970</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>

</xml_diff>

<commit_message>
calc logic fixed. routing added.
</commit_message>
<xml_diff>
--- a/spraycalc.xlsx
+++ b/spraycalc.xlsx
@@ -5,12 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Statisch" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Dynamisch" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Beispiel" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Calc" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t xml:space="preserve">Liter</t>
   </si>
@@ -79,9 +78,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -113,7 +113,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,14 +134,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD4EA6B"/>
-        <bgColor rgb="FFCCFFCC"/>
+        <fgColor rgb="FFE8F2A1"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB4C7DC"/>
         <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD4EA6B"/>
+        <bgColor rgb="FFE8F2A1"/>
       </patternFill>
     </fill>
   </fills>
@@ -179,7 +185,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -200,6 +206,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -208,11 +222,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -261,8 +295,8 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFD4EA6B"/>
+      <rgbColor rgb="FFE8F2A1"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
@@ -296,10 +330,10 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -458,13 +492,15 @@
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.39"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -474,7 +510,7 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -488,49 +524,45 @@
       <c r="C2" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <f aca="false">B2/C2</f>
-        <v>200</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="5" t="n">
         <v>200</v>
       </c>
-      <c r="C3" s="5" t="n">
+      <c r="C3" s="6" t="n">
         <f aca="false">B3/B2*C2</f>
         <v>1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <f aca="false">B3/C3</f>
-        <v>200</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="7" t="n">
         <f aca="false">B2-B3</f>
         <v>1800</v>
       </c>
-      <c r="C4" s="6" t="n">
+      <c r="C4" s="7" t="n">
         <f aca="false">C2-C3</f>
         <v>9</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="8" t="n">
         <f aca="false">B4/C4</f>
         <v>200</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+    </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="10" t="s">
         <v>0</v>
       </c>
     </row>
@@ -538,12 +570,12 @@
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="n">
-        <f aca="false">B4/C4-SUM(B8:B13)</f>
+      <c r="B7" s="11" t="n">
+        <f aca="false">D4-SUM(B8:B13)</f>
         <v>179</v>
       </c>
-      <c r="C7" s="5" t="n">
-        <f aca="false">B7*$C$4</f>
+      <c r="C7" s="11" t="n">
+        <f aca="false">$C$4*B7</f>
         <v>1611</v>
       </c>
     </row>
@@ -551,11 +583,11 @@
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="n">
+      <c r="B8" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="5" t="n">
-        <f aca="false">B8*$C$4</f>
+      <c r="C8" s="11" t="n">
+        <f aca="false">$C$4*B8</f>
         <v>9</v>
       </c>
     </row>
@@ -563,11 +595,11 @@
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="n">
+      <c r="B9" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="5" t="n">
-        <f aca="false">B9*$C$4</f>
+      <c r="C9" s="11" t="n">
+        <f aca="false">$C$4*B9</f>
         <v>18</v>
       </c>
     </row>
@@ -575,11 +607,11 @@
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="n">
+      <c r="B10" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="C10" s="5" t="n">
-        <f aca="false">B10*$C$4</f>
+      <c r="C10" s="11" t="n">
+        <f aca="false">$C$4*B10</f>
         <v>27</v>
       </c>
     </row>
@@ -587,11 +619,11 @@
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="n">
+      <c r="B11" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="C11" s="5" t="n">
-        <f aca="false">B11*$C$4</f>
+      <c r="C11" s="11" t="n">
+        <f aca="false">$C$4*B11</f>
         <v>36</v>
       </c>
     </row>
@@ -599,11 +631,11 @@
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="7" t="n">
+      <c r="B12" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="C12" s="5" t="n">
-        <f aca="false">B12*$C$4</f>
+      <c r="C12" s="11" t="n">
+        <f aca="false">$C$4*B12</f>
         <v>45</v>
       </c>
     </row>
@@ -611,242 +643,36 @@
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="7" t="n">
+      <c r="B13" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="C13" s="5" t="n">
-        <f aca="false">B13*$C$4</f>
+      <c r="C13" s="11" t="n">
+        <f aca="false">$C$4*B13</f>
         <v>54</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="8" t="n">
+      <c r="B14" s="13" t="n">
         <f aca="false">SUM(B7:B13)</f>
         <v>200</v>
       </c>
-      <c r="C14" s="8" t="n">
+      <c r="C14" s="13" t="n">
         <f aca="false">SUM(C7:C13)</f>
         <v>1800</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D20"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.4"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>3300</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>280</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <f aca="false">B2/C2</f>
-        <v>11.7857142857143</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>330</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <f aca="false">B3/B2*C2</f>
-        <v>28</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <f aca="false">B3/C3</f>
-        <v>11.7857142857143</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="6" t="n">
-        <f aca="false">B2-B3</f>
-        <v>2970</v>
-      </c>
-      <c r="C4" s="6" t="n">
-        <f aca="false">C2-C3</f>
-        <v>252</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <f aca="false">B4/C4</f>
-        <v>11.7857142857143</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="n">
-        <f aca="false">C4-SUM(B8:B13)</f>
-        <v>231</v>
-      </c>
-      <c r="C7" s="5" t="n">
-        <f aca="false">B7*$D$4</f>
-        <v>2722.5</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="5" t="n">
-        <f aca="false">B8*$D$4</f>
-        <v>11.7857142857143</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" s="5" t="n">
-        <f aca="false">B9*$D$4</f>
-        <v>23.5714285714286</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C10" s="5" t="n">
-        <f aca="false">B10*$D$4</f>
-        <v>35.3571428571429</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="C11" s="5" t="n">
-        <f aca="false">B11*$D$4</f>
-        <v>47.1428571428571</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C12" s="5" t="n">
-        <f aca="false">B12*$D$4</f>
-        <v>58.9285714285714</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C13" s="5" t="n">
-        <f aca="false">B13*$D$4</f>
-        <v>70.7142857142857</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="8" t="n">
-        <f aca="false">SUM(B7:B13)</f>
-        <v>252</v>
-      </c>
-      <c r="C14" s="8" t="n">
-        <f aca="false">SUM(C7:C13)</f>
-        <v>2970</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="15" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>